<commit_message>
PHQ parameter calculation done
</commit_message>
<xml_diff>
--- a/Project/Electrified Reactor/parameters.xlsx
+++ b/Project/Electrified Reactor/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\repos_python\Project\Electrified Reactor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C9745E-F36E-431A-B284-4964606B783C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D50351-289D-42FA-9A06-23D477465FE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>t</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +86,22 @@
   </si>
   <si>
     <t>CS Tavg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0D Tmax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0D Tavg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fitted Tmax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fitted Tavg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5189,15 +5205,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A19B01-1174-4447-A637-16FB1E66919D}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5211,19 +5231,31 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.01</v>
       </c>
@@ -5237,19 +5269,31 @@
         <v>767.4</v>
       </c>
       <c r="E2">
+        <v>954.4</v>
+      </c>
+      <c r="F2">
+        <v>767.4</v>
+      </c>
+      <c r="G2">
         <v>0.70532271999999996</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>4.1978469999999997E-2</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>955</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>768.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>951.6</v>
+      </c>
+      <c r="L2">
+        <v>765.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.01</v>
       </c>
@@ -5263,19 +5307,31 @@
         <v>792.7</v>
       </c>
       <c r="E3">
+        <v>1140.3</v>
+      </c>
+      <c r="F3">
+        <v>792.7</v>
+      </c>
+      <c r="G3">
         <v>0.50279980000000002</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>3.2738700000000003E-2</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>1132.9000000000001</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>793.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>1111.5999999999999</v>
+      </c>
+      <c r="L3">
+        <v>797.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.01</v>
       </c>
@@ -5289,19 +5345,31 @@
         <v>820.8</v>
       </c>
       <c r="E4">
+        <v>1324.3</v>
+      </c>
+      <c r="F4">
+        <v>820.8</v>
+      </c>
+      <c r="G4">
         <v>0.43933242</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>2.8612149999999999E-2</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>1320.3</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>822.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>1271.3</v>
+      </c>
+      <c r="L4">
+        <v>833.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.01</v>
       </c>
@@ -5315,19 +5383,31 @@
         <v>876</v>
       </c>
       <c r="E5">
+        <v>1480.1</v>
+      </c>
+      <c r="F5">
+        <v>876</v>
+      </c>
+      <c r="G5">
         <v>0.43206550999999999</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>2.1869179999999998E-2</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>1479.6</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>879.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>1423.6</v>
+      </c>
+      <c r="L5">
+        <v>870.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -5341,19 +5421,31 @@
         <v>908.8</v>
       </c>
       <c r="E6">
+        <v>1627.5</v>
+      </c>
+      <c r="F6">
+        <v>908.8</v>
+      </c>
+      <c r="G6">
         <v>0.43714094999999997</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>2.1590560000000002E-2</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>1628.4</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>912.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>1580.6</v>
+      </c>
+      <c r="L6">
+        <v>909.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.01</v>
       </c>
@@ -5367,19 +5459,31 @@
         <v>982.6</v>
       </c>
       <c r="E7">
+        <v>1827.8</v>
+      </c>
+      <c r="F7">
+        <v>982.6</v>
+      </c>
+      <c r="G7">
         <v>0.42645124000000001</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>1.806089E-2</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>1822.9</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>986.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>1747.9</v>
+      </c>
+      <c r="L7">
+        <v>950.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.01</v>
       </c>
@@ -5392,20 +5496,32 @@
       <c r="D8">
         <v>998.4</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
+        <v>1947.8</v>
+      </c>
+      <c r="F8">
+        <v>998.4</v>
+      </c>
+      <c r="G8" s="1">
         <v>0.45082712000000003</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H8" s="1">
         <v>1.9999240000000001E-2</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>1949.8</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>1004.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>1927.7</v>
+      </c>
+      <c r="L8">
+        <v>993.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.01</v>
       </c>
@@ -5418,20 +5534,32 @@
       <c r="D9">
         <v>1003.2</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
+        <v>2025.6</v>
+      </c>
+      <c r="F9">
+        <v>1003.2</v>
+      </c>
+      <c r="G9" s="1">
         <v>0.49105293</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <v>2.2837059999999999E-2</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>2023.9</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>1009</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>2121</v>
+      </c>
+      <c r="L9">
+        <v>1039.5999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.02</v>
       </c>
@@ -5444,20 +5572,32 @@
       <c r="D10">
         <v>769.6</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
+        <v>1018.5</v>
+      </c>
+      <c r="F10">
+        <v>769.6</v>
+      </c>
+      <c r="G10" s="1">
         <v>1.0030676300000001</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>7.5498270000000006E-2</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>1017.6</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>770.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>1018.7</v>
+      </c>
+      <c r="L10">
+        <v>769.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.02</v>
       </c>
@@ -5470,20 +5610,32 @@
       <c r="D11">
         <v>821.1</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
+        <v>1235.8</v>
+      </c>
+      <c r="F11">
+        <v>821.1</v>
+      </c>
+      <c r="G11" s="1">
         <v>0.79065830999999998</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <v>4.4544790000000001E-2</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>1233.2</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>823.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>1253.9000000000001</v>
+      </c>
+      <c r="L11">
+        <v>825.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.02</v>
       </c>
@@ -5496,20 +5648,32 @@
       <c r="D12">
         <v>917.3</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
+        <v>1453.4</v>
+      </c>
+      <c r="F12">
+        <v>917.3</v>
+      </c>
+      <c r="G12" s="1">
         <v>0.73298279</v>
       </c>
-      <c r="F12" s="1">
+      <c r="H12" s="1">
         <v>2.7778170000000001E-2</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>1443</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>918.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>1543.1</v>
+      </c>
+      <c r="L12">
+        <v>891.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.02</v>
       </c>
@@ -5522,20 +5686,32 @@
       <c r="D13">
         <v>979.1</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
+        <v>1748.5</v>
+      </c>
+      <c r="F13">
+        <v>979.1</v>
+      </c>
+      <c r="G13" s="1">
         <v>0.65754561</v>
       </c>
-      <c r="F13" s="1">
+      <c r="H13" s="1">
         <v>2.6565600000000002E-2</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>1740.3</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>982.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <v>1809.5</v>
+      </c>
+      <c r="L13">
+        <v>958.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0.02</v>
       </c>
@@ -5548,20 +5724,32 @@
       <c r="D14">
         <v>1014</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
+        <v>1988.1</v>
+      </c>
+      <c r="F14">
+        <v>1014</v>
+      </c>
+      <c r="G14" s="1">
         <v>0.65517417</v>
       </c>
-      <c r="F14" s="1">
+      <c r="H14" s="1">
         <v>2.8921840000000001E-2</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>1985.1</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>1020.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <v>2081</v>
+      </c>
+      <c r="L14">
+        <v>1028.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>0.06</v>
       </c>
@@ -5574,20 +5762,32 @@
       <c r="D15">
         <v>800.4</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="F15">
+        <v>800.4</v>
+      </c>
+      <c r="G15" s="1">
         <v>1.5122611399999999</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <v>0.10179361000000001</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>1136.5999999999999</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>802</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <v>1140.3</v>
+      </c>
+      <c r="L15">
+        <v>800.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>0.06</v>
       </c>
@@ -5600,20 +5800,32 @@
       <c r="D16">
         <v>899.3</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
+        <v>1487.3</v>
+      </c>
+      <c r="F16">
+        <v>899.3</v>
+      </c>
+      <c r="G16" s="1">
         <v>1.2356109900000001</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <v>6.055779E-2</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>1483.1</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>903</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>1476.5</v>
+      </c>
+      <c r="L16">
+        <v>899.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>0.06</v>
       </c>
@@ -5626,21 +5838,34 @@
       <c r="D17">
         <v>990.1</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
+        <v>1816.2</v>
+      </c>
+      <c r="F17">
+        <v>990.1</v>
+      </c>
+      <c r="G17" s="1">
         <v>1.18414255</v>
       </c>
-      <c r="F17" s="1">
+      <c r="H17" s="1">
         <v>5.345573E-2</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>1809.6</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>995.6</v>
+      </c>
+      <c r="K17">
+        <v>1802.2</v>
+      </c>
+      <c r="L17">
+        <v>993.3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>